<commit_message>
migratet to new version ESPAsyncWebServer. Added some error handling for more stability
</commit_message>
<xml_diff>
--- a/CV Rechner.xlsx
+++ b/CV Rechner.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Andy\Repos\NMRA-DCC\cDecoder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70666B40-121A-41FD-96CE-F255F9421919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{74FF30BB-A00B-4517-B187-14A215E5B478}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11565" yWindow="4680" windowWidth="28800" windowHeight="15345" xr2:uid="{F033B1C5-6916-4DC7-B96D-A2CCF64752B7}"/>
+    <workbookView minimized="1" xWindow="7575" yWindow="2625" windowWidth="21225" windowHeight="15345" xr2:uid="{F033B1C5-6916-4DC7-B96D-A2CCF64752B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,7 +420,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -429,7 +430,7 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>6019</v>
+        <v>6018</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -447,7 +448,7 @@
       </c>
       <c r="B4">
         <f>B1-((B3-192)*256)</f>
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>